<commit_message>
refactor diagram and documentation of user
</commit_message>
<xml_diff>
--- a/docs/Cronograma de Actividades - Roberto siles.xlsx
+++ b/docs/Cronograma de Actividades - Roberto siles.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Registro de Usuarios</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Diseño del diagrama de clases</t>
   </si>
   <si>
-    <t>29/09/17</t>
-  </si>
-  <si>
     <t>Implementar el diagrama de la base de datos</t>
   </si>
   <si>
@@ -68,23 +65,38 @@
     <t>Implementacion de los CRUDS necesarios del lado del Cliente</t>
   </si>
   <si>
-    <t>30/10/17</t>
-  </si>
-  <si>
     <t>Sincronizar el servidor con el cliente</t>
   </si>
   <si>
-    <t>20/10/17</t>
-  </si>
-  <si>
     <t>Corregir Bugs si hubiera</t>
+  </si>
+  <si>
+    <t>26/09/17</t>
+  </si>
+  <si>
+    <t>29/09/2017</t>
+  </si>
+  <si>
+    <t>28/09/2017</t>
+  </si>
+  <si>
+    <t>16/10/17</t>
+  </si>
+  <si>
+    <t>17/10/2017</t>
+  </si>
+  <si>
+    <t>19/10/2017</t>
+  </si>
+  <si>
+    <t>20/10/2017</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +106,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -136,18 +155,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -467,12 +487,14 @@
   <dimension ref="B2:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="1" max="4" width="11.5546875" style="3"/>
+    <col min="5" max="5" width="20.21875" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" x14ac:dyDescent="0.3">
@@ -496,12 +518,12 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
       <c r="F3" s="2">
         <v>2</v>
       </c>
@@ -511,177 +533,152 @@
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="4">
-        <v>42776</v>
-      </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="4">
-        <v>42835</v>
+      <c r="H5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="J5" s="4">
-        <v>42835</v>
+      <c r="J5" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="2"/>
-      <c r="H6" s="4">
-        <v>42896</v>
+      <c r="H6" s="5">
+        <v>42776</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="J6" s="4">
-        <v>42896</v>
+      <c r="J6" s="5">
+        <v>42776</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="4">
+      <c r="H7" s="5">
+        <v>42804</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="5">
         <v>42988</v>
       </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="2">
         <v>5</v>
       </c>
       <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
+      <c r="H8" s="5">
+        <v>43018</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="2">
         <v>2</v>
       </c>
       <c r="G9" s="2"/>
-      <c r="H9" s="4">
-        <v>42746</v>
+      <c r="H9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="J9" s="4">
-        <v>42897</v>
+      <c r="J9" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="2">
         <v>2</v>
       </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="4">
-        <v>42958</v>
+      <c r="H10" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="I10" s="2"/>
-      <c r="J10" s="4">
-        <v>43080</v>
+      <c r="J10" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="K10" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -693,6 +690,31 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="H4:I4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J8:K8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>